<commit_message>
adding size class as a fish obs
</commit_message>
<xml_diff>
--- a/data-raw/metadata/fish_observations_metadata.xlsx
+++ b/data-raw/metadata/fish_observations_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddeerubenson/Documents/git/VA/edi-feather-snorkel/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EEDDB12-4830-0D40-BCB0-09680E1E3C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD272F2B-DB92-F540-A9DD-4A618815FAC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30160" yWindow="800" windowWidth="34640" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="57">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -148,9 +148,6 @@
     <t>If adipose fin is clipped (TRUE, FALSE)</t>
   </si>
   <si>
-    <t>Fork length of observed fish</t>
-  </si>
-  <si>
     <t xml:space="preserve">observation_id           </t>
   </si>
   <si>
@@ -181,17 +178,26 @@
     <t>Fish species observed based on visual observation</t>
   </si>
   <si>
-    <t xml:space="preserve">Substrate associated with observation. If multiple substrates are observed at one site, all substrate types are reccorded. Levels = c( 1- Fine, 2- Small/medium gravel, 3- Medium/large cobble, 4- Boulder, 5- Pavement, NA). Value is NA when no fish is observed. </t>
+    <t xml:space="preserve">Instream cover associated with observation. If multiple cover types are observed at one observation site, all cover types are reccorded. Types of cover include: E - Submerged Aquatic Veg/Algae, B - Small Instream Objects/Woody Debris, C - Large Instream Objects/Woody Debris, A - No apparent Cover, F - undercut bank. Value is NA when no fish is observed. </t>
   </si>
   <si>
-    <t xml:space="preserve">Instream cover associated with observation. If multiple cover types are observed at one site, all cover types are reccorded. Types of cover include: E - Submerged Aquatic Veg/Algae, B - Small Instream Objects/Woody Debris, C - Large Instream Objects/Woody Debris, A - No apparent Cover, F - undercut bank. Value is NA when no fish is observed. </t>
+    <t xml:space="preserve">Overhead cover associated with observation.  If multiple cover types are observed at one site, all cover types are reccorded. Types of cover include: 0 - no apparent cover, 1 - overhead object/veg 0 - 0.5 meters, 2 - overhead object/veg 0.5 - 2 meters, 3 - submerged aquatic veg/algae. Value is NA when no fish are is observed. </t>
   </si>
   <si>
-    <t xml:space="preserve">Overhead cover associated with observation.  If multiple cover types are observed at one site, all cover types are reccorded. Types of cover include: 0 - no apparent cover, 1 - overhead object/veg 0 - 0.5 meters, 2 - overhead object/veg 0.5 - 2 meters, 3 - submerged aquatic veg/algae. Value is NA when no fish is observed. </t>
+    <t>Channel geomorphology associated with observation. Levels = c(backwater, glide, glide margin, pool, riffle, riffle margin, NA). Value is NA when no fish is observed. 
+)</t>
   </si>
   <si>
-    <t>Channel geomorphology associated with observation. Levels = c("backwater", "glide", "glide margin", "pool", "riffle", "riffle margin", NA). Value is NA when no fish is observed. 
-)</t>
+    <t>Fork length of observed fish. Size class range (I - 0-50 mm, II - 51-75 mm, III - 76-100 mm, IV - 101-150 mm, V - 151-300 mm, VI - 301-499 mm, VII - 500+ mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Substrate associated with observation. If multiple substrates are observed at one site, all substrate types are reccorded. Levels = c( 1- Organic Fines, Mud (0.05 mm) 2- Sand (0.05 to 2 mm), 3- Small Gravel (2 to 50 mm), 4- Large Gravel (50 to 150 mm), 5-Cobble (150 to 300 mm), 6-Boulder (&gt;300 mm), NA). Value is NA when no fish is observed. </t>
+  </si>
+  <si>
+    <t>size_class</t>
+  </si>
+  <si>
+    <t>Size class range (I - 0-50 mm, II - 51-75 mm, III - 76-100 mm, IV - 101-150 mm, V - 151-300 mm, VI - 301-499 mm, VII - 500+ mm)</t>
   </si>
 </sst>
 </file>
@@ -202,7 +208,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -223,6 +229,13 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -261,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -300,6 +313,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,17 +530,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z972"/>
+  <dimension ref="A1:Z973"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
-    <col min="2" max="2" width="42" style="15" customWidth="1"/>
+    <col min="2" max="2" width="55.83203125" style="15" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" customWidth="1"/>
@@ -543,7 +558,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -595,10 +610,10 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>34</v>
@@ -636,7 +651,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>34</v>
@@ -674,7 +689,7 @@
         <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
@@ -760,7 +775,7 @@
         <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -797,8 +812,8 @@
       <c r="A7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>40</v>
+      <c r="B7" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>15</v>
@@ -843,10 +858,10 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>39</v>
+      <c r="B8" s="14" t="s">
+        <v>56</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>13</v>
@@ -865,26 +880,26 @@
       <c r="K8" s="2"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
-      <c r="W8" s="1"/>
-      <c r="X8" s="1"/>
-      <c r="Y8" s="1"/>
-      <c r="Z8" s="1"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="17"/>
+      <c r="U8" s="17"/>
+      <c r="V8" s="17"/>
+      <c r="W8" s="17"/>
+      <c r="X8" s="17"/>
+      <c r="Y8" s="17"/>
+      <c r="Z8" s="17"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -919,10 +934,10 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>52</v>
+      <c r="B10" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>
@@ -957,10 +972,10 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
@@ -995,10 +1010,10 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
@@ -1033,38 +1048,28 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
       <c r="I13" s="2"/>
       <c r="J13" s="3"/>
       <c r="K13" s="2"/>
-      <c r="L13" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="M13" s="11">
-        <v>5</v>
-      </c>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -1081,10 +1086,10 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>15</v>
@@ -1099,7 +1104,7 @@
         <v>15</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>17</v>
@@ -1127,33 +1132,53 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
-      <c r="T20" s="1"/>
-      <c r="U20" s="1"/>
-      <c r="V20" s="1"/>
-      <c r="W20" s="1"/>
-      <c r="X20" s="1"/>
-      <c r="Y20" s="1"/>
-      <c r="Z20" s="1"/>
+    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="M15" s="11">
+        <v>5</v>
+      </c>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
@@ -1884,7 +1909,7 @@
       <c r="Z46" s="1"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="1"/>
+      <c r="A47" s="4"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="2"/>
@@ -27811,18 +27836,46 @@
       <c r="Y972" s="1"/>
       <c r="Z972" s="1"/>
     </row>
+    <row r="973" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A973" s="1"/>
+      <c r="B973" s="1"/>
+      <c r="C973" s="1"/>
+      <c r="D973" s="2"/>
+      <c r="E973" s="1"/>
+      <c r="F973" s="3"/>
+      <c r="G973" s="3"/>
+      <c r="H973" s="3"/>
+      <c r="I973" s="2"/>
+      <c r="J973" s="3"/>
+      <c r="K973" s="2"/>
+      <c r="L973" s="3"/>
+      <c r="M973" s="3"/>
+      <c r="N973" s="1"/>
+      <c r="O973" s="1"/>
+      <c r="P973" s="1"/>
+      <c r="Q973" s="1"/>
+      <c r="R973" s="1"/>
+      <c r="S973" s="1"/>
+      <c r="T973" s="1"/>
+      <c r="U973" s="1"/>
+      <c r="V973" s="1"/>
+      <c r="W973" s="1"/>
+      <c r="X973" s="1"/>
+      <c r="Y973" s="1"/>
+      <c r="Z973" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C29:C972 C1:C14" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C30:C973 C1:C7 C9:C15" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E20:E972 E1:E14" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E21:E973 E1:E7 E9:E15" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F20:F972 F1:F14" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F21:F973 F1:F7 F9:F15" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H20:H972 H1:H14" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H21:H973 H1:H7 H9:H15" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
adds date to fish obs, tries to fill in survey type, changes section name to lower and removes NA dates
</commit_message>
<xml_diff>
--- a/data-raw/metadata/fish_observations_metadata.xlsx
+++ b/data-raw/metadata/fish_observations_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddeerubenson/Documents/git/VA/edi-feather-snorkel/data-raw/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/edi-feather-snorkel/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD272F2B-DB92-F540-A9DD-4A618815FAC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212C2F30-FAFD-5D45-B1F6-871E530C3895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30160" yWindow="800" windowWidth="34640" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -199,14 +199,27 @@
   <si>
     <t>Size class range (I - 0-50 mm, II - 51-75 mm, III - 76-100 mm, IV - 101-150 mm, V - 151-300 mm, VI - 301-499 mm, VII - 500+ mm)</t>
   </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Date of survey event</t>
+  </si>
+  <si>
+    <t>dateTime</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -274,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -313,8 +326,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,11 +548,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z973"/>
+  <dimension ref="A1:Z974"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -558,7 +576,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -686,28 +704,34 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>47</v>
+      <c r="B4" s="17" t="s">
+        <v>58</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="5"/>
+      <c r="J4" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="K4" s="6"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="3"/>
+      <c r="L4" s="18">
+        <v>36259</v>
+      </c>
+      <c r="M4" s="18">
+        <v>44099</v>
+      </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -724,38 +748,28 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>37</v>
-      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
       <c r="I5" s="2"/>
       <c r="J5" s="5"/>
       <c r="K5" s="6"/>
-      <c r="L5" s="9">
-        <v>0</v>
-      </c>
-      <c r="M5" s="12">
-        <v>30000</v>
-      </c>
+      <c r="L5" s="9"/>
+      <c r="M5" s="3"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -772,28 +786,38 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="I6" s="2"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="9">
+        <v>0</v>
+      </c>
+      <c r="M6" s="12">
+        <v>30000</v>
+      </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -810,38 +834,28 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>53</v>
+      <c r="B7" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
       <c r="I7" s="2"/>
       <c r="J7" s="3"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="3">
-        <v>0</v>
-      </c>
-      <c r="M7" s="3">
-        <v>900</v>
-      </c>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -858,48 +872,58 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>56</v>
+      <c r="B8" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="I8" s="2"/>
       <c r="J8" s="3"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="17"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="17"/>
-      <c r="U8" s="17"/>
-      <c r="V8" s="17"/>
-      <c r="W8" s="17"/>
-      <c r="X8" s="17"/>
-      <c r="Y8" s="17"/>
-      <c r="Z8" s="17"/>
+      <c r="L8" s="3">
+        <v>0</v>
+      </c>
+      <c r="M8" s="3">
+        <v>900</v>
+      </c>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>39</v>
+      <c r="B9" s="14" t="s">
+        <v>56</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -918,26 +942,26 @@
       <c r="K9" s="2"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
-      <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="16"/>
+      <c r="V9" s="16"/>
+      <c r="W9" s="16"/>
+      <c r="X9" s="16"/>
+      <c r="Y9" s="16"/>
+      <c r="Z9" s="16"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>54</v>
+      <c r="B10" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>
@@ -972,10 +996,10 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>50</v>
+      <c r="B11" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
@@ -1010,10 +1034,10 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
@@ -1048,10 +1072,10 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>13</v>
@@ -1086,38 +1110,28 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>17</v>
-      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
       <c r="I14" s="2"/>
       <c r="J14" s="3"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="M14" s="11">
-        <v>5</v>
-      </c>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -1134,10 +1148,10 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>15</v>
@@ -1152,7 +1166,7 @@
         <v>15</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>17</v>
@@ -1180,33 +1194,53 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
-      <c r="T21" s="1"/>
-      <c r="U21" s="1"/>
-      <c r="V21" s="1"/>
-      <c r="W21" s="1"/>
-      <c r="X21" s="1"/>
-      <c r="Y21" s="1"/>
-      <c r="Z21" s="1"/>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="M16" s="11">
+        <v>5</v>
+      </c>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
@@ -1937,7 +1971,7 @@
       <c r="Z47" s="1"/>
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="1"/>
+      <c r="A48" s="4"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="2"/>
@@ -27864,18 +27898,46 @@
       <c r="Y973" s="1"/>
       <c r="Z973" s="1"/>
     </row>
+    <row r="974" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A974" s="1"/>
+      <c r="B974" s="1"/>
+      <c r="C974" s="1"/>
+      <c r="D974" s="2"/>
+      <c r="E974" s="1"/>
+      <c r="F974" s="3"/>
+      <c r="G974" s="3"/>
+      <c r="H974" s="3"/>
+      <c r="I974" s="2"/>
+      <c r="J974" s="3"/>
+      <c r="K974" s="2"/>
+      <c r="L974" s="3"/>
+      <c r="M974" s="3"/>
+      <c r="N974" s="1"/>
+      <c r="O974" s="1"/>
+      <c r="P974" s="1"/>
+      <c r="Q974" s="1"/>
+      <c r="R974" s="1"/>
+      <c r="S974" s="1"/>
+      <c r="T974" s="1"/>
+      <c r="U974" s="1"/>
+      <c r="V974" s="1"/>
+      <c r="W974" s="1"/>
+      <c r="X974" s="1"/>
+      <c r="Y974" s="1"/>
+      <c r="Z974" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C30:C973 C1:C7 C9:C15" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C31:C974 C10:C16 C1:C8" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E21:E973 E1:E7 E9:E15" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E22:E974 E10:E16 E1:E8" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F21:F973 F1:F7 F9:F15" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F22:F974 F10:F16 F1:F8" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H21:H973 H1:H7 H9:H15" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H22:H974 H10:H16 H1:H8" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updates xml will need to be updated on main branch
</commit_message>
<xml_diff>
--- a/data-raw/metadata/fish_observations_metadata.xlsx
+++ b/data-raw/metadata/fish_observations_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/edi-feather-snorkel/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212C2F30-FAFD-5D45-B1F6-871E530C3895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D283D4F-F111-0941-8089-EE50E322EF34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30160" yWindow="800" windowWidth="34640" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1440" windowWidth="28800" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="60">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -128,9 +128,6 @@
   </si>
   <si>
     <t>meter</t>
-  </si>
-  <si>
-    <t>ordinal</t>
   </si>
   <si>
     <t>snorkel_survey</t>
@@ -551,8 +548,8 @@
   <dimension ref="A1:Z974"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -628,16 +625,16 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>14</v>
@@ -669,13 +666,13 @@
         <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>14</v>
@@ -704,26 +701,26 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="C4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="2"/>
       <c r="J4" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K4" s="6"/>
       <c r="L4" s="18">
@@ -751,13 +748,13 @@
         <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
@@ -795,7 +792,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>16</v>
@@ -804,10 +801,10 @@
         <v>15</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="5"/>
@@ -837,13 +834,13 @@
         <v>30</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>14</v>
@@ -875,13 +872,13 @@
         <v>31</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>16</v>
@@ -920,16 +917,16 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>14</v>
@@ -961,13 +958,13 @@
         <v>27</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>14</v>
@@ -999,13 +996,13 @@
         <v>24</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>14</v>
@@ -1037,13 +1034,13 @@
         <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>14</v>
@@ -1075,13 +1072,13 @@
         <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>14</v>
@@ -1110,16 +1107,16 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>14</v>
@@ -1148,16 +1145,16 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>16</v>
@@ -1196,16 +1193,16 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>16</v>
@@ -1214,7 +1211,7 @@
         <v>15</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
fixes issues in eml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/fish_observations_metadata.xlsx
+++ b/data-raw/metadata/fish_observations_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/edi-feather-snorkel/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D283D4F-F111-0941-8089-EE50E322EF34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6585FB5-647C-8E4D-8ACB-6E33C5AE32AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1440" windowWidth="28800" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="520" windowWidth="28800" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="59">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -128,9 +128,6 @@
   </si>
   <si>
     <t>meter</t>
-  </si>
-  <si>
-    <t>snorkel_survey</t>
   </si>
   <si>
     <t>count of fish</t>
@@ -548,8 +545,8 @@
   <dimension ref="A1:Z974"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -625,17 +622,15 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="1" t="s">
         <v>14</v>
       </c>
@@ -666,14 +661,12 @@
         <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
@@ -701,26 +694,24 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="C4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="2"/>
       <c r="J4" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K4" s="6"/>
       <c r="L4" s="18">
@@ -748,14 +739,12 @@
         <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
@@ -791,9 +780,7 @@
       <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="1" t="s">
         <v>16</v>
       </c>
@@ -801,10 +788,10 @@
         <v>15</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="5"/>
@@ -834,14 +821,12 @@
         <v>30</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="D7" s="2"/>
       <c r="E7" s="1" t="s">
         <v>14</v>
       </c>
@@ -872,14 +857,12 @@
         <v>31</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="1" t="s">
         <v>16</v>
       </c>
@@ -917,17 +900,15 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="1" t="s">
         <v>14</v>
       </c>
@@ -958,14 +939,12 @@
         <v>27</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="D10" s="2"/>
       <c r="E10" s="1" t="s">
         <v>14</v>
       </c>
@@ -996,14 +975,12 @@
         <v>24</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="1" t="s">
         <v>14</v>
       </c>
@@ -1034,14 +1011,12 @@
         <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="1" t="s">
         <v>14</v>
       </c>
@@ -1072,14 +1047,12 @@
         <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1107,17 +1080,15 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="D14" s="2"/>
       <c r="E14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1145,17 +1116,15 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="D15" s="2"/>
       <c r="E15" s="1" t="s">
         <v>16</v>
       </c>
@@ -1193,17 +1162,15 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1211,7 +1178,7 @@
         <v>15</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
updates to methods mostly
</commit_message>
<xml_diff>
--- a/data-raw/metadata/fish_observations_metadata.xlsx
+++ b/data-raw/metadata/fish_observations_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/edi-feather-snorkel/data-raw/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddeerubenson/Documents/git/VA/edi-feather-snorkel/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212C2F30-FAFD-5D45-B1F6-871E530C3895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856EB73A-985F-1447-B5B6-20DEA6921FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30160" yWindow="800" windowWidth="34640" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -552,7 +552,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updates the xml and metadata with updated min and max
</commit_message>
<xml_diff>
--- a/data-raw/metadata/fish_observations_metadata.xlsx
+++ b/data-raw/metadata/fish_observations_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddeerubenson/Documents/git/VA/edi-feather-snorkel/data-raw/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/edi-feather-snorkel/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856EB73A-985F-1447-B5B6-20DEA6921FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D2C32B-0169-BF44-B453-4090509B047C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="60">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -128,9 +128,6 @@
   </si>
   <si>
     <t>meter</t>
-  </si>
-  <si>
-    <t>ordinal</t>
   </si>
   <si>
     <t>snorkel_survey</t>
@@ -550,9 +547,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z974"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -628,16 +625,16 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>14</v>
@@ -669,13 +666,13 @@
         <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>14</v>
@@ -704,33 +701,33 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="C4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="2"/>
       <c r="J4" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K4" s="6"/>
       <c r="L4" s="18">
-        <v>36259</v>
+        <v>36297</v>
       </c>
       <c r="M4" s="18">
-        <v>44099</v>
+        <v>45128</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -751,13 +748,13 @@
         <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
@@ -795,7 +792,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>16</v>
@@ -804,10 +801,10 @@
         <v>15</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="5"/>
@@ -816,7 +813,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="12">
-        <v>30000</v>
+        <v>50000</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -837,13 +834,13 @@
         <v>30</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>14</v>
@@ -875,13 +872,13 @@
         <v>31</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>16</v>
@@ -902,7 +899,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="3">
-        <v>900</v>
+        <v>1524</v>
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
@@ -920,16 +917,16 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>14</v>
@@ -961,13 +958,13 @@
         <v>27</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>14</v>
@@ -999,13 +996,13 @@
         <v>24</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>14</v>
@@ -1037,13 +1034,13 @@
         <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>14</v>
@@ -1075,13 +1072,13 @@
         <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>14</v>
@@ -1110,16 +1107,16 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>14</v>
@@ -1148,16 +1145,16 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>16</v>
@@ -1175,7 +1172,7 @@
       <c r="J15" s="3"/>
       <c r="K15" s="2"/>
       <c r="L15" s="11">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="M15" s="11">
         <v>5</v>
@@ -1196,16 +1193,16 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>16</v>
@@ -1214,7 +1211,7 @@
         <v>15</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>17</v>
@@ -1226,7 +1223,7 @@
         <v>0.05</v>
       </c>
       <c r="M16" s="11">
-        <v>5</v>
+        <v>5.85</v>
       </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>

</xml_diff>